<commit_message>
more documentation/comments for t-test program
</commit_message>
<xml_diff>
--- a/T-Test Results.xlsx
+++ b/T-Test Results.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanyakhattar/Desktop/HPV/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanyakhattar/Desktop/HPV/HPVResearch/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="500" windowWidth="24720" windowHeight="16580" tabRatio="500"/>
+    <workbookView xWindow="14920" yWindow="500" windowWidth="15320" windowHeight="16580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Section 1" sheetId="1" r:id="rId1"/>
@@ -252,7 +252,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -271,6 +271,21 @@
     <font>
       <sz val="12"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -302,7 +317,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -328,11 +343,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -614,8 +640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="81" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -722,35 +748,35 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="12">
         <v>-3.9316661440699199</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="16">
         <v>9.4903123256971303E-5</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="4">
+      <c r="G4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="12">
         <v>319</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="12">
         <v>554</v>
       </c>
     </row>
@@ -783,99 +809,99 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="12">
         <v>-2.65846120985081</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="16">
         <v>8.0281657206980207E-3</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="4">
+      <c r="G6" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="12">
         <v>408</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="12">
         <v>554</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="12">
         <v>2.2882910073255802</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="12">
         <v>2.52030880964778E-2</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="4">
+      <c r="G7" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="12">
         <v>408</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="12">
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="12">
         <v>3.7292800600896201</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="16">
         <v>3.9851364915772603E-4</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" s="4">
+      <c r="G8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="12">
         <v>554</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8" s="12">
         <v>66</v>
       </c>
     </row>
@@ -1299,33 +1325,33 @@
       </c>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
+    <row r="25" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D25" s="8">
+      <c r="D25" s="13">
         <v>1.99413238306326</v>
       </c>
-      <c r="E25" s="8">
+      <c r="E25" s="13">
         <v>4.7200215475140403E-2</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="F25" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G25" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4">
+      <c r="G25" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12">
         <v>221</v>
       </c>
-      <c r="J25" s="4">
+      <c r="J25" s="12">
         <v>1025</v>
       </c>
     </row>
@@ -1744,7 +1770,7 @@
       <c r="G43" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H43" s="10"/>
+      <c r="H43" s="9"/>
       <c r="I43" s="4">
         <v>171</v>
       </c>
@@ -1775,35 +1801,35 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A45" s="4" t="s">
+    <row r="45" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C45" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D45" s="4">
+      <c r="D45" s="12">
         <f>2.25483330564737</f>
         <v>2.2548333056473702</v>
       </c>
-      <c r="E45" s="4">
+      <c r="E45" s="12">
         <f>0.0246602071965265</f>
         <v>2.46602071965265E-2</v>
       </c>
-      <c r="F45" s="4" t="s">
+      <c r="F45" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G45" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H45" s="10"/>
-      <c r="I45" s="4">
+      <c r="G45" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H45" s="14"/>
+      <c r="I45" s="12">
         <v>304</v>
       </c>
-      <c r="J45" s="4">
+      <c r="J45" s="12">
         <v>598</v>
       </c>
     </row>
@@ -1833,7 +1859,7 @@
       <c r="J46" s="1"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A47" s="11" t="s">
+      <c r="A47" s="10" t="s">
         <v>49</v>
       </c>
       <c r="B47" s="4" t="s">
@@ -1855,7 +1881,7 @@
       <c r="G47" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H47" s="10"/>
+      <c r="H47" s="9"/>
       <c r="I47" s="4">
         <v>598</v>
       </c>
@@ -1889,7 +1915,7 @@
       <c r="J48" s="1"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A49" s="11" t="s">
+      <c r="A49" s="10" t="s">
         <v>54</v>
       </c>
       <c r="B49" s="4" t="s">
@@ -1910,7 +1936,7 @@
       <c r="G49" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H49" s="10"/>
+      <c r="H49" s="9"/>
       <c r="I49" s="4" t="s">
         <v>67</v>
       </c>
@@ -1968,38 +1994,38 @@
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C52" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="D52" s="8">
+      <c r="D52" s="13">
         <v>-2.7103743356068</v>
       </c>
-      <c r="E52" s="8">
+      <c r="E52" s="13">
         <v>7.3304718845403696E-3</v>
       </c>
-      <c r="F52" s="8" t="s">
+      <c r="F52" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="G52" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H52" s="10"/>
-      <c r="I52" s="4" t="s">
+      <c r="G52" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H52" s="14"/>
+      <c r="I52" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="J52" s="4" t="s">
+      <c r="J52" s="12" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A53" s="11" t="s">
+      <c r="A53" s="10" t="s">
         <v>58</v>
       </c>
       <c r="B53" s="4" t="s">
@@ -2020,7 +2046,7 @@
       <c r="G53" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="H53" s="10"/>
+      <c r="H53" s="9"/>
       <c r="I53" s="4" t="s">
         <v>71</v>
       </c>

</xml_diff>